<commit_message>
Aerospace Factory & Aerospace Electronics
</commit_message>
<xml_diff>
--- a/OBL comparison.xlsx
+++ b/OBL comparison.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Propulsion Factory Q3" sheetId="6" r:id="rId1"/>
+    <sheet name="Aerospace Factory Q3" sheetId="7" r:id="rId2"/>
+    <sheet name="Aerospace Electronics Q3 " sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t>Alphas</t>
   </si>
@@ -147,6 +149,63 @@
   </si>
   <si>
     <t>Rocket Fuel</t>
+  </si>
+  <si>
+    <t>Fuselage</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>Propellant tank</t>
+  </si>
+  <si>
+    <t>Heat shield</t>
+  </si>
+  <si>
+    <t>Sub-Orbital 2nd stage</t>
+  </si>
+  <si>
+    <t>Orbital Booster</t>
+  </si>
+  <si>
+    <t>Starship</t>
+  </si>
+  <si>
+    <t>Carbon Composite</t>
+  </si>
+  <si>
+    <t>Silicon</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Flight computer</t>
+  </si>
+  <si>
+    <t>cockpit</t>
+  </si>
+  <si>
+    <t>Attitude control</t>
+  </si>
+  <si>
+    <t>Quadcopter</t>
+  </si>
+  <si>
+    <t>Satellite</t>
+  </si>
+  <si>
+    <t>On-board computer</t>
+  </si>
+  <si>
+    <t>Displays</t>
+  </si>
+  <si>
+    <t>Basic interior</t>
+  </si>
+  <si>
+    <t>Plastic</t>
   </si>
 </sst>
 </file>
@@ -212,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -334,12 +393,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -371,11 +467,20 @@
     <xf numFmtId="44" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -465,6 +570,168 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12340167" y="6529917"/>
+          <a:ext cx="984250" cy="414791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>486833</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>664095</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>178796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12545483" y="5972174"/>
+          <a:ext cx="4301587" cy="483597"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118458</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12471400" y="5580592"/>
+          <a:ext cx="984250" cy="414791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>486833</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>664095</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>7346</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13612283" y="5972174"/>
+          <a:ext cx="4301587" cy="483597"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>118458</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13538200" y="5580592"/>
           <a:ext cx="984250" cy="414791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -743,7 +1010,7 @@
   <dimension ref="A2:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +1076,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="3">
-        <v>18.899999999999999</v>
+        <v>19.2</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>21</v>
@@ -940,11 +1207,11 @@
       </c>
       <c r="D18" s="26">
         <f>30*B6+100*B9+50*B8</f>
-        <v>4802</v>
+        <v>4811</v>
       </c>
       <c r="E18" s="26">
         <f>20*B4+8*B5+10*B6</f>
-        <v>7405</v>
+        <v>7408</v>
       </c>
       <c r="F18" s="26">
         <f>8*B5+30*B10+15*B8</f>
@@ -952,7 +1219,7 @@
       </c>
       <c r="G18" s="26">
         <f>4*B5+5*B6</f>
-        <v>3594.5</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -969,11 +1236,11 @@
       </c>
       <c r="D19" s="27">
         <f t="shared" si="0"/>
-        <v>4802</v>
+        <v>4811</v>
       </c>
       <c r="E19" s="27">
         <f t="shared" si="0"/>
-        <v>7405</v>
+        <v>7408</v>
       </c>
       <c r="F19" s="27">
         <f t="shared" si="0"/>
@@ -981,7 +1248,7 @@
       </c>
       <c r="G19" s="27">
         <f t="shared" si="0"/>
-        <v>3594.5</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1018,35 +1285,35 @@
       <c r="A23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="36">
         <v>78</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="31">
         <v>232</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <v>645</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>9700</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31">
         <v>11550</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="31">
         <v>11550</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="31">
         <v>5400</v>
       </c>
     </row>
@@ -1054,40 +1321,40 @@
       <c r="A25" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="33">
+      <c r="B25" s="35">
         <v>0.05</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="33">
+      <c r="B26" s="35">
         <v>0.25</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="31">
+      <c r="B27" s="36">
         <v>0</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
@@ -1103,11 +1370,11 @@
       </c>
       <c r="D28" s="29">
         <f t="shared" si="2"/>
-        <v>2058.8943577430982</v>
+        <v>2049.8943577430982</v>
       </c>
       <c r="E28" s="29">
         <f t="shared" si="2"/>
-        <v>1305.8943577430982</v>
+        <v>1302.8943577430982</v>
       </c>
       <c r="F28" s="29">
         <f t="shared" si="2"/>
@@ -1115,7 +1382,7 @@
       </c>
       <c r="G28" s="29">
         <f t="shared" si="2"/>
-        <v>859.13145258103214</v>
+        <v>857.63145258103214</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1161,11 +1428,11 @@
       </c>
       <c r="D30" s="29">
         <f t="shared" si="4"/>
-        <v>7641.1056422569018</v>
+        <v>7650.1056422569018</v>
       </c>
       <c r="E30" s="29">
         <f t="shared" si="4"/>
-        <v>10244.105642256902</v>
+        <v>10247.105642256902</v>
       </c>
       <c r="F30" s="29">
         <f t="shared" si="4"/>
@@ -1173,7 +1440,7 @@
       </c>
       <c r="G30" s="29">
         <f t="shared" si="4"/>
-        <v>4540.8685474189679</v>
+        <v>4542.3685474189679</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1181,27 +1448,27 @@
         <v>24</v>
       </c>
       <c r="B31" s="16">
-        <f>B30-B19-B20</f>
+        <f t="shared" ref="B31:G31" si="5">B30-B19-B20</f>
         <v>5.6513833603616845</v>
       </c>
       <c r="C31" s="16">
-        <f>C30-C19-C20</f>
+        <f t="shared" si="5"/>
         <v>31.062424969988015</v>
       </c>
       <c r="D31" s="16">
-        <f>D30-D19-D20</f>
+        <f t="shared" si="5"/>
         <v>621.24849939975911</v>
       </c>
       <c r="E31" s="16">
-        <f>E30-E19-E20</f>
+        <f t="shared" si="5"/>
         <v>621.24849939975911</v>
       </c>
       <c r="F31" s="16">
-        <f>F30-F19-F20</f>
+        <f t="shared" si="5"/>
         <v>310.62424969987956</v>
       </c>
       <c r="G31" s="16">
-        <f>G30-G19-G20</f>
+        <f t="shared" si="5"/>
         <v>207.08283313325353</v>
       </c>
     </row>
@@ -1214,24 +1481,24 @@
         <v>1136496.7058823549</v>
       </c>
       <c r="C32" s="12">
-        <f t="shared" ref="C32:G32" si="5">(C24-C19-C20*(1-0.03*$B$27)*(1+$B$23/170*(1-$B$26))*(1-$B$25))*$B$23*C16/(1-$B$25)*24</f>
+        <f t="shared" ref="C32:G32" si="6">(C24-C19-C20*(1-0.03*$B$27)*(1+$B$23/170*(1-$B$26))*(1-$B$25))*$B$23*C16/(1-$B$25)*24</f>
         <v>944587.14798761567</v>
       </c>
       <c r="D32" s="12">
-        <f t="shared" si="5"/>
-        <v>1139905.716408669</v>
+        <f t="shared" si="6"/>
+        <v>1134939.9900928796</v>
       </c>
       <c r="E32" s="12">
-        <f t="shared" si="5"/>
-        <v>724439.94798761629</v>
+        <f t="shared" si="6"/>
+        <v>722784.70588235313</v>
       </c>
       <c r="F32" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>331595.82167182682</v>
       </c>
       <c r="G32" s="12">
-        <f t="shared" si="5"/>
-        <v>1425986.7269349841</v>
+        <f t="shared" si="6"/>
+        <v>1423503.8637770896</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1240,28 +1507,28 @@
         <v>25</v>
       </c>
       <c r="B35" s="22">
-        <f>((B24-B19)*(1+B25)/B20-1)*170/2/(1-B26)</f>
+        <f t="shared" ref="B35:G35" si="7">((B24-B19)*(1+B25)/B20-1)*170/2/(1-B26)</f>
         <v>149.13927536231904</v>
       </c>
       <c r="C35" s="22">
-        <f>((C24-C19)*(1+C25)/C20-1)*170/2/(1-C26)</f>
+        <f t="shared" si="7"/>
         <v>89.150080515297873</v>
       </c>
       <c r="D35" s="22">
-        <f>((D24-D19)*(1+D25)/D20-1)*170/2/(1-D26)</f>
-        <v>102.71723027375201</v>
+        <f t="shared" si="7"/>
+        <v>102.37230273752016</v>
       </c>
       <c r="E35" s="22">
-        <f>((E24-E19)*(1+E25)/E20-1)*170/2/(1-E26)</f>
-        <v>73.858293075684401</v>
+        <f t="shared" si="7"/>
+        <v>73.74331723027376</v>
       </c>
       <c r="F35" s="22">
-        <f>((F24-F19)*(1+F25)/F20-1)*170/2/(1-F26)</f>
+        <f t="shared" si="7"/>
         <v>46.570692431562016</v>
       </c>
       <c r="G35" s="22">
-        <f>((G24-G19)*(1+G25)/G20-1)*170/2/(1-G26)</f>
-        <v>122.58888888888887</v>
+        <f t="shared" si="7"/>
+        <v>122.41642512077296</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1273,24 +1540,24 @@
         <v>1475413.0768252218</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36:G36" si="6">(C24-C19-C20*(1-0.03*$B$27)*(1+C35/170*(1-$B$26))*(1-$B$25))*C35*C16/(1-$B$25)*24</f>
+        <f t="shared" ref="C36:G36" si="8">(C24-C19-C20*(1-0.03*$B$27)*(1+C35/170*(1-$B$26))*(1-$B$25))*C35*C16/(1-$B$25)*24</f>
         <v>1014255.2108599029</v>
       </c>
       <c r="D36" s="12">
-        <f t="shared" si="6"/>
-        <v>1334188.4816089503</v>
+        <f t="shared" si="8"/>
+        <v>1325512.6964739391</v>
       </c>
       <c r="E36" s="12">
-        <f t="shared" si="6"/>
-        <v>706086.83671497647</v>
+        <f t="shared" si="8"/>
+        <v>703980.25387439667</v>
       </c>
       <c r="F36" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>294224.22260055959</v>
       </c>
       <c r="G36" s="12">
-        <f t="shared" si="6"/>
-        <v>1881743.186631578</v>
+        <f t="shared" si="8"/>
+        <v>1876587.3566864992</v>
       </c>
     </row>
   </sheetData>
@@ -1340,4 +1607,1187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L36"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="15">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3">
+        <v>19.2</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3">
+        <v>35</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="3">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="24">
+        <v>3.48</v>
+      </c>
+      <c r="C16" s="24">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="D16" s="24">
+        <v>4.74</v>
+      </c>
+      <c r="E16" s="24">
+        <v>12.65</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="25">
+        <v>587</v>
+      </c>
+      <c r="C17" s="25">
+        <v>587</v>
+      </c>
+      <c r="D17" s="25">
+        <v>587</v>
+      </c>
+      <c r="E17" s="25">
+        <v>587</v>
+      </c>
+      <c r="F17" s="25">
+        <v>587</v>
+      </c>
+      <c r="G17" s="25">
+        <v>587</v>
+      </c>
+      <c r="H17" s="25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="26">
+        <f>40*B4</f>
+        <v>2756</v>
+      </c>
+      <c r="C18" s="26">
+        <f>30*B4+5*B5</f>
+        <v>2163</v>
+      </c>
+      <c r="D18" s="26">
+        <f>50*B5+250*B6</f>
+        <v>9710</v>
+      </c>
+      <c r="E18" s="26">
+        <f>20*B8+30*B7</f>
+        <v>453</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+    </row>
+    <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="27">
+        <f>B18</f>
+        <v>2756</v>
+      </c>
+      <c r="C19" s="27">
+        <f t="shared" ref="C19:H19" si="0">C18</f>
+        <v>2163</v>
+      </c>
+      <c r="D19" s="27">
+        <f t="shared" si="0"/>
+        <v>9710</v>
+      </c>
+      <c r="E19" s="27">
+        <f t="shared" si="0"/>
+        <v>453</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="28">
+        <f>B17/B16</f>
+        <v>168.67816091954023</v>
+      </c>
+      <c r="C20" s="28">
+        <f t="shared" ref="C20:H20" si="1">C17/C16</f>
+        <v>68.735362997658086</v>
+      </c>
+      <c r="D20" s="28">
+        <f t="shared" si="1"/>
+        <v>123.83966244725738</v>
+      </c>
+      <c r="E20" s="28">
+        <f t="shared" si="1"/>
+        <v>46.403162055335969</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="28" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="36">
+        <v>78</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="31">
+        <v>3080</v>
+      </c>
+      <c r="C24" s="31">
+        <v>2210</v>
+      </c>
+      <c r="D24" s="31">
+        <v>9500</v>
+      </c>
+      <c r="E24" s="31">
+        <v>600</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="36">
+        <v>0</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="29">
+        <f>B24-B30</f>
+        <v>108.0730545091601</v>
+      </c>
+      <c r="C28" s="29">
+        <f t="shared" ref="C28:H28" si="2">C24-C30</f>
+        <v>-40.988966078234625</v>
+      </c>
+      <c r="D28" s="29">
+        <f t="shared" si="2"/>
+        <v>-368.52864352491997</v>
+      </c>
+      <c r="E28" s="29">
+        <f t="shared" si="2"/>
+        <v>87.598753335326251</v>
+      </c>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H28" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="30">
+        <f>$B$23*B16*24*(1+$B$25)</f>
+        <v>6840.2879999999996</v>
+      </c>
+      <c r="C29" s="30">
+        <f t="shared" ref="C29:H29" si="3">$B$23*C16*24*(1+$B$25)</f>
+        <v>16786.223999999998</v>
+      </c>
+      <c r="D29" s="30">
+        <f t="shared" si="3"/>
+        <v>9316.9440000000013</v>
+      </c>
+      <c r="E29" s="30">
+        <f t="shared" si="3"/>
+        <v>24864.840000000004</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="29">
+        <f>B19+B20*(1+$B$23/170*(1-$B$26))/(1+$B$25)</f>
+        <v>2971.9269454908399</v>
+      </c>
+      <c r="C30" s="29">
+        <f t="shared" ref="C30:H30" si="4">C19+C20*(1+$B$23/170*(1-$B$26))/(1+$B$25)</f>
+        <v>2250.9889660782346</v>
+      </c>
+      <c r="D30" s="29">
+        <f t="shared" si="4"/>
+        <v>9868.52864352492</v>
+      </c>
+      <c r="E30" s="29">
+        <f t="shared" si="4"/>
+        <v>512.40124666467375</v>
+      </c>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="29" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="16">
+        <f t="shared" ref="B31:H31" si="5">B30-B19-B20</f>
+        <v>47.248784571299666</v>
+      </c>
+      <c r="C31" s="16">
+        <f t="shared" si="5"/>
+        <v>19.253603080576539</v>
+      </c>
+      <c r="D31" s="16">
+        <f t="shared" si="5"/>
+        <v>34.688981077662589</v>
+      </c>
+      <c r="E31" s="16">
+        <f t="shared" si="5"/>
+        <v>12.998084609337781</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="16" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="12">
+        <f>(B24-B19-B20*(1-0.03*$B$27)*(1+$B$23/170*(1-$B$26))*(1-$B$25))*$B$23*B16/(1-$B$25)*24</f>
+        <v>744805.33746130019</v>
+      </c>
+      <c r="C32" s="12">
+        <f t="shared" ref="C32:H32" si="6">(C24-C19-C20*(1-0.03*$B$27)*(1+$B$23/170*(1-$B$26))*(1-$B$25))*$B$23*C16/(1-$B$25)*24</f>
+        <v>-686072.64148606826</v>
+      </c>
+      <c r="D32" s="12">
+        <f t="shared" si="6"/>
+        <v>-3438464.3888544897</v>
+      </c>
+      <c r="E32" s="12">
+        <f t="shared" si="6"/>
+        <v>2187289.716408669</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H32" s="12" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="22">
+        <f t="shared" ref="B35:H35" si="7">((B24-B19)*(1+B25)/B20-1)*170/2/(1-B26)</f>
+        <v>115.24397501419647</v>
+      </c>
+      <c r="C35" s="22">
+        <f t="shared" si="7"/>
+        <v>-26.878534923339018</v>
+      </c>
+      <c r="D35" s="22">
+        <f t="shared" si="7"/>
+        <v>-229.13798977853492</v>
+      </c>
+      <c r="E35" s="22">
+        <f t="shared" si="7"/>
+        <v>184.27044293015331</v>
+      </c>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H35" s="22" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="12">
+        <f>(B24-B19-B20*(1-0.03*$B$27)*(1+B35/170*(1-$B$26))*(1-$B$25))*B35*B16/(1-$B$25)*24</f>
+        <v>833670.74220770749</v>
+      </c>
+      <c r="C36" s="12">
+        <f t="shared" ref="C36:H36" si="8">(C24-C19-C20*(1-0.03*$B$27)*(1+C35/170*(1-$B$26))*(1-$B$25))*C35*C16/(1-$B$25)*24</f>
+        <v>61210.317821752004</v>
+      </c>
+      <c r="D36" s="12">
+        <f t="shared" si="8"/>
+        <v>5726925.3738366356</v>
+      </c>
+      <c r="E36" s="12">
+        <f t="shared" si="8"/>
+        <v>3950234.0955045745</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H36" s="12" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:H27"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B36:H36">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:H35">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:H32">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J39"/>
+  <sheetViews>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="15">
+        <v>875</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3">
+        <v>456</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3">
+        <v>119</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3">
+        <v>55.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3">
+        <v>11550</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="24">
+        <v>2.38</v>
+      </c>
+      <c r="C19" s="24">
+        <v>2.38</v>
+      </c>
+      <c r="D19" s="24">
+        <v>2.86</v>
+      </c>
+      <c r="E19" s="24">
+        <v>13.1</v>
+      </c>
+      <c r="F19" s="24">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="25">
+        <v>725</v>
+      </c>
+      <c r="C20" s="25">
+        <v>725</v>
+      </c>
+      <c r="D20" s="25">
+        <v>725</v>
+      </c>
+      <c r="E20" s="25">
+        <v>725</v>
+      </c>
+      <c r="F20" s="25">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="26">
+        <f>B4*4+2*B5</f>
+        <v>4412</v>
+      </c>
+      <c r="C21" s="26">
+        <f>4*B4+8*B6+1*B7</f>
+        <v>4762</v>
+      </c>
+      <c r="D21" s="26">
+        <f>3*B8+5*B9+3*B10</f>
+        <v>1156.4000000000001</v>
+      </c>
+      <c r="E21" s="26">
+        <f>B5+B9+3*B11+2*B12</f>
+        <v>731.69999999999993</v>
+      </c>
+      <c r="F21" s="26">
+        <f>4*B27+B13+8*B4+2*D27</f>
+        <v>42170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="27">
+        <f>B21</f>
+        <v>4412</v>
+      </c>
+      <c r="C22" s="27">
+        <f t="shared" ref="C22:F22" si="0">C21</f>
+        <v>4762</v>
+      </c>
+      <c r="D22" s="27">
+        <f t="shared" si="0"/>
+        <v>1156.4000000000001</v>
+      </c>
+      <c r="E22" s="27">
+        <f t="shared" si="0"/>
+        <v>731.69999999999993</v>
+      </c>
+      <c r="F22" s="27">
+        <f t="shared" si="0"/>
+        <v>42170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="28">
+        <f>B20/B19</f>
+        <v>304.62184873949582</v>
+      </c>
+      <c r="C23" s="28">
+        <f t="shared" ref="C23:F23" si="1">C20/C19</f>
+        <v>304.62184873949582</v>
+      </c>
+      <c r="D23" s="28">
+        <f t="shared" si="1"/>
+        <v>253.49650349650352</v>
+      </c>
+      <c r="E23" s="28">
+        <f t="shared" si="1"/>
+        <v>55.343511450381683</v>
+      </c>
+      <c r="F23" s="28">
+        <f t="shared" si="1"/>
+        <v>6041.666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="32">
+        <v>78</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="31">
+        <v>5040</v>
+      </c>
+      <c r="C27" s="31">
+        <v>5400</v>
+      </c>
+      <c r="D27" s="31">
+        <v>1730</v>
+      </c>
+      <c r="E27" s="31">
+        <v>855</v>
+      </c>
+      <c r="F27" s="31">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="36">
+        <v>0</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="29">
+        <f>B27-B33</f>
+        <v>238.04990231386637</v>
+      </c>
+      <c r="C31" s="29">
+        <f t="shared" ref="C31:F31" si="2">C27-C33</f>
+        <v>248.04990231386637</v>
+      </c>
+      <c r="D31" s="29">
+        <f t="shared" si="2"/>
+        <v>249.09607255489595</v>
+      </c>
+      <c r="E31" s="29">
+        <f t="shared" si="2"/>
+        <v>52.454104389847657</v>
+      </c>
+      <c r="F31" s="29">
+        <f t="shared" si="2"/>
+        <v>2095.9897292250243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="30">
+        <f>$B$26*B19*24*(1+$B$28)</f>
+        <v>4678.1279999999997</v>
+      </c>
+      <c r="C32" s="30">
+        <f>$B$26*C19*24*(1+$B$28)</f>
+        <v>4678.1279999999997</v>
+      </c>
+      <c r="D32" s="30">
+        <f>$B$26*D19*24*(1+$B$28)</f>
+        <v>5621.616</v>
+      </c>
+      <c r="E32" s="30">
+        <f>$B$26*E19*24*(1+$B$28)</f>
+        <v>25749.359999999997</v>
+      </c>
+      <c r="F32" s="30">
+        <f>$B$26*F19*24*(1+$B$28)</f>
+        <v>235.87199999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="29">
+        <f>B22+B23*(1+$B$26/170*(1-$B$29))/(1+$B$28)</f>
+        <v>4801.9500976861336</v>
+      </c>
+      <c r="C33" s="29">
+        <f>C22+C23*(1+$B$26/170*(1-$B$29))/(1+$B$28)</f>
+        <v>5151.9500976861336</v>
+      </c>
+      <c r="D33" s="29">
+        <f>D22+D23*(1+$B$26/170*(1-$B$29))/(1+$B$28)</f>
+        <v>1480.903927445104</v>
+      </c>
+      <c r="E33" s="29">
+        <f>E22+E23*(1+$B$26/170*(1-$B$29))/(1+$B$28)</f>
+        <v>802.54589561015234</v>
+      </c>
+      <c r="F33" s="29">
+        <f>F22+F23*(1+$B$26/170*(1-$B$29))/(1+$B$28)</f>
+        <v>49904.010270774976</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="16">
+        <f t="shared" ref="B34:F34" si="3">B33-B22-B23</f>
+        <v>85.328248946637814</v>
+      </c>
+      <c r="C34" s="16">
+        <f t="shared" si="3"/>
+        <v>85.328248946637814</v>
+      </c>
+      <c r="D34" s="16">
+        <f t="shared" si="3"/>
+        <v>71.007423948600433</v>
+      </c>
+      <c r="E34" s="16">
+        <f t="shared" si="3"/>
+        <v>15.502384159770727</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="3"/>
+        <v>1692.3436041083087</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="12">
+        <f>(B27-B22-B23*(1-0.03*$B$30)*(1+$B$26/170*(1-$B$29))*(1-$B$28))*$B$26*B19/(1-$B$28)*24</f>
+        <v>1120990.9820433436</v>
+      </c>
+      <c r="C35" s="12">
+        <f>(C27-C22-C23*(1-0.03*$B$30)*(1+$B$26/170*(1-$B$29))*(1-$B$28))*$B$26*C19/(1-$B$28)*24</f>
+        <v>1167889.5083591328</v>
+      </c>
+      <c r="D35" s="12">
+        <f>(D27-D22-D23*(1-0.03*$B$30)*(1+$B$26/170*(1-$B$29))*(1-$B$28))*$B$26*D19/(1-$B$28)*24</f>
+        <v>1408404.0683591326</v>
+      </c>
+      <c r="E35" s="12">
+        <f>(E27-E22-E23*(1-0.03*$B$30)*(1+$B$26/170*(1-$B$29))*(1-$B$28))*$B$26*E19/(1-$B$28)*24</f>
+        <v>1358616.7504643979</v>
+      </c>
+      <c r="F35" s="12">
+        <f>(F27-F22-F23*(1-0.03*$B$30)*(1+$B$26/170*(1-$B$29))*(1-$B$28))*$B$26*F19/(1-$B$28)*24</f>
+        <v>500196.37151702779</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="22">
+        <f t="shared" ref="B38:F38" si="4">((B27-B22)*(1+B28)/B23-1)*170/2/(1-B29)</f>
+        <v>131.99378390804597</v>
+      </c>
+      <c r="C38" s="22">
+        <f t="shared" si="4"/>
+        <v>93.023999999999987</v>
+      </c>
+      <c r="D38" s="22">
+        <f t="shared" si="4"/>
+        <v>107.3340137931034</v>
+      </c>
+      <c r="E38" s="22">
+        <f t="shared" si="4"/>
+        <v>104.37179310344835</v>
+      </c>
+      <c r="F38" s="22">
+        <f t="shared" si="4"/>
+        <v>53.297931034482744</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="12">
+        <f>(B27-B22-B23*(1-0.03*$B$30)*(1+B38/170*(1-$B$29))*(1-$B$28))*B38*B19/(1-$B$28)*24</f>
+        <v>1349882.2545676546</v>
+      </c>
+      <c r="C39" s="12">
+        <f>(C27-C22-C23*(1-0.03*$B$30)*(1+C38/170*(1-$B$29))*(1-$B$28))*C38*C19/(1-$B$28)*24</f>
+        <v>1285557.2121599996</v>
+      </c>
+      <c r="D39" s="12">
+        <f>(D27-D22-D23*(1-0.03*$B$30)*(1+D38/170*(1-$B$29))*(1-$B$28))*D38*D19/(1-$B$28)*24</f>
+        <v>1696376.03526753</v>
+      </c>
+      <c r="E39" s="12">
+        <f>(E27-E22-E23*(1-0.03*$B$30)*(1+E38/170*(1-$B$29))*(1-$B$28))*E38*E19/(1-$B$28)*24</f>
+        <v>1606672.3013008016</v>
+      </c>
+      <c r="F39" s="12">
+        <f>(F27-F22-F23*(1-0.03*$B$30)*(1+F38/170*(1-$B$29))*(1-$B$28))*F38*F19/(1-$B$28)*24</f>
+        <v>442853.63102722313</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B39:F39">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38:F38">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:F35">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>